<commit_message>
Fontstyle fixed for the first sheet
</commit_message>
<xml_diff>
--- a/testfile2.xlsx
+++ b/testfile2.xlsx
@@ -19,13 +19,25 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="1">
+  <fonts count="3">
     <font>
       <sz val="11.0"/>
       <color indexed="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <sz val="9.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <sz val="9.0"/>
+      <color indexed="8"/>
+      <b val="true"/>
     </font>
   </fonts>
   <fills count="2">
@@ -48,8 +60,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="true"/>
   </cellXfs>
 </styleSheet>
 </file>
@@ -63,19 +77,19 @@
   <sheetFormatPr defaultRowHeight="15.0"/>
   <sheetData>
     <row r="1">
-      <c r="A1" t="inlineStr">
+      <c r="A1" s="2" t="inlineStr">
         <is>
           <t>RUBRIK</t>
         </is>
       </c>
-      <c r="B1" t="inlineStr">
+      <c r="B1" s="2" t="inlineStr">
         <is>
           <t>INNEHÅLL</t>
         </is>
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="inlineStr">
+      <c r="A2" s="1" t="inlineStr">
         <is>
           <t>Riksarkivets diarienummer leveransöverenskommelse</t>
         </is>
@@ -83,7 +97,7 @@
       <c r="B2"/>
     </row>
     <row r="3">
-      <c r="A3" t="inlineStr">
+      <c r="A3" s="1" t="inlineStr">
         <is>
           <t>Riksarkivets diarienummer leverans</t>
         </is>
@@ -91,7 +105,7 @@
       <c r="B3"/>
     </row>
     <row r="4">
-      <c r="A4" t="inlineStr">
+      <c r="A4" s="2" t="inlineStr">
         <is>
           <t>Beskrivning av leveransen</t>
         </is>
@@ -99,7 +113,7 @@
       <c r="B4"/>
     </row>
     <row r="5">
-      <c r="A5" t="inlineStr">
+      <c r="A5" s="2" t="inlineStr">
         <is>
           <t>Arkivbildare</t>
         </is>
@@ -107,7 +121,7 @@
       <c r="B5"/>
     </row>
     <row r="6">
-      <c r="A6" t="inlineStr">
+      <c r="A6" s="2" t="inlineStr">
         <is>
           <t>Organisationsnummer arkivbildare</t>
         </is>
@@ -115,7 +129,7 @@
       <c r="B6"/>
     </row>
     <row r="7">
-      <c r="A7" t="inlineStr">
+      <c r="A7" s="2" t="inlineStr">
         <is>
           <t>Levererande myndighet</t>
         </is>
@@ -123,7 +137,7 @@
       <c r="B7"/>
     </row>
     <row r="8">
-      <c r="A8" t="inlineStr">
+      <c r="A8" s="2" t="inlineStr">
         <is>
           <t>Organisationsnummer levererande myndighet</t>
         </is>
@@ -131,7 +145,7 @@
       <c r="B8"/>
     </row>
     <row r="9">
-      <c r="A9" t="inlineStr">
+      <c r="A9" s="2" t="inlineStr">
         <is>
           <t>Servicebyrå/Konsult</t>
         </is>
@@ -139,7 +153,7 @@
       <c r="B9"/>
     </row>
     <row r="10">
-      <c r="A10" t="inlineStr">
+      <c r="A10" s="2" t="inlineStr">
         <is>
           <t>Kontaktperson för leverans</t>
         </is>
@@ -147,7 +161,7 @@
       <c r="B10"/>
     </row>
     <row r="11">
-      <c r="A11" t="inlineStr">
+      <c r="A11" s="2" t="inlineStr">
         <is>
           <t>Telefonnummer till kontaktperson</t>
         </is>
@@ -155,7 +169,7 @@
       <c r="B11"/>
     </row>
     <row r="12">
-      <c r="A12" t="inlineStr">
+      <c r="A12" s="2" t="inlineStr">
         <is>
           <t>Kostnadsställe</t>
         </is>
@@ -163,7 +177,7 @@
       <c r="B12"/>
     </row>
     <row r="13">
-      <c r="A13" t="inlineStr">
+      <c r="A13" s="1" t="inlineStr">
         <is>
           <t>Kontaktperson för e-fakturering</t>
         </is>
@@ -171,7 +185,7 @@
       <c r="B13"/>
     </row>
     <row r="14">
-      <c r="A14" t="inlineStr">
+      <c r="A14" s="1" t="inlineStr">
         <is>
           <t>Arkivets namn</t>
         </is>
@@ -179,7 +193,7 @@
       <c r="B14"/>
     </row>
     <row r="15">
-      <c r="A15" t="inlineStr">
+      <c r="A15" s="2" t="inlineStr">
         <is>
           <t>Systemets namn</t>
         </is>
@@ -187,7 +201,7 @@
       <c r="B15"/>
     </row>
     <row r="16">
-      <c r="A16" t="inlineStr">
+      <c r="A16" s="2" t="inlineStr">
         <is>
           <t>Uttagsdatum</t>
         </is>
@@ -195,7 +209,7 @@
       <c r="B16"/>
     </row>
     <row r="17">
-      <c r="A17" t="inlineStr">
+      <c r="A17" s="2" t="inlineStr">
         <is>
           <t>Kommentar</t>
         </is>
@@ -203,7 +217,7 @@
       <c r="B17"/>
     </row>
     <row r="18">
-      <c r="A18" t="inlineStr">
+      <c r="A18" s="2" t="inlineStr">
         <is>
           <t>Projektkod</t>
         </is>
@@ -211,7 +225,7 @@
       <c r="B18"/>
     </row>
     <row r="19">
-      <c r="A19" t="inlineStr">
+      <c r="A19" s="1" t="inlineStr">
         <is>
           <t>Accessions-ID</t>
         </is>
@@ -219,7 +233,7 @@
       <c r="B19"/>
     </row>
     <row r="20">
-      <c r="A20" t="inlineStr">
+      <c r="A20" s="1" t="inlineStr">
         <is>
           <t>Batch-ID</t>
         </is>
@@ -294,12 +308,12 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>.DS_Store</t>
+          <t>Argumenterande_Tal_NP14.doc</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>DS_Store</t>
+          <t>doc</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
@@ -309,7 +323,7 @@
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>8196</t>
+          <t>17408</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
@@ -324,7 +338,7 @@
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>TestFiles</t>
+          <t>Svenska</t>
         </is>
       </c>
       <c r="H2" t="inlineStr">
@@ -346,12 +360,12 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>.DS_Store</t>
+          <t>Argumenter_Text.doc</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>DS_Store</t>
+          <t>doc</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
@@ -361,7 +375,7 @@
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>6148</t>
+          <t>20992</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
@@ -376,7 +390,7 @@
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>TestFiles/OE</t>
+          <t>Svenska</t>
         </is>
       </c>
       <c r="H3" t="inlineStr">
@@ -398,12 +412,12 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>.DS_Store</t>
+          <t>ENG_ArEs_CLCH.doc</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>DS_Store</t>
+          <t>doc</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
@@ -413,7 +427,7 @@
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>6148</t>
+          <t>10240</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
@@ -428,7 +442,7 @@
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>TestFiles/subfolder</t>
+          <t>Svenska</t>
         </is>
       </c>
       <c r="H4" t="inlineStr">
@@ -450,12 +464,12 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Harry_Potter_and_the_Goblet_of_Fire_2005.mkv</t>
+          <t>Filmanalys.doc</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>mkv</t>
+          <t>doc</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
@@ -465,7 +479,7 @@
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>443051505</t>
+          <t>10240</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
@@ -475,12 +489,12 @@
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>02:37:06</t>
+          <t/>
         </is>
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>TestFiles/movies</t>
+          <t>Svenska</t>
         </is>
       </c>
       <c r="H5" t="inlineStr">
@@ -502,12 +516,12 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Lucifer.S02E04.HDTV.x264-LOL[eztv].mkv</t>
+          <t>Maskrosen_Milad.doc</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>mkv</t>
+          <t>doc</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
@@ -517,7 +531,7 @@
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>324677395</t>
+          <t>15360</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
@@ -527,12 +541,12 @@
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>00:42:15</t>
+          <t/>
         </is>
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>TestFiles/movies</t>
+          <t>Svenska</t>
         </is>
       </c>
       <c r="H6" t="inlineStr">
@@ -554,12 +568,12 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Skaermavbild_2018-02-19_kl._22.57.05.png</t>
+          <t>Namnlös 1.doc</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>png</t>
+          <t>doc</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
@@ -569,7 +583,7 @@
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>2460165</t>
+          <t>9216</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
@@ -584,7 +598,7 @@
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>TestFiles/subfolder/another_subfolder</t>
+          <t>Svenska</t>
         </is>
       </c>
       <c r="H7" t="inlineStr">
@@ -606,12 +620,12 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>AEAEAEAEAE.txt</t>
+          <t>Novell_Analys.doc</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>txt</t>
+          <t>doc</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
@@ -621,12 +635,12 @@
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>16384</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>UTF-8</t>
+          <t/>
         </is>
       </c>
       <c r="F8" t="inlineStr">
@@ -636,7 +650,7 @@
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>TestFiles</t>
+          <t>Svenska</t>
         </is>
       </c>
       <c r="H8" t="inlineStr">
@@ -658,12 +672,12 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>aaaaaaaaaa.txt</t>
+          <t>Språk_Och_Makt.doc</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>txt</t>
+          <t>doc</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
@@ -673,12 +687,12 @@
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>27</t>
+          <t>16384</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>UTF-8</t>
+          <t/>
         </is>
       </c>
       <c r="F9" t="inlineStr">
@@ -688,7 +702,7 @@
       </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t>TestFiles/OE/aa</t>
+          <t>Svenska</t>
         </is>
       </c>
       <c r="H9" t="inlineStr">
@@ -710,12 +724,12 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>oeaeoeaeoeaeoeae.txt</t>
+          <t>inlamning_2_Saikat.doc</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>txt</t>
+          <t>doc</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
@@ -725,12 +739,12 @@
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>22</t>
+          <t>9216</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>UTF-8</t>
+          <t/>
         </is>
       </c>
       <c r="F10" t="inlineStr">
@@ -740,7 +754,7 @@
       </c>
       <c r="G10" t="inlineStr">
         <is>
-          <t>TestFiles/OE</t>
+          <t>Svenska\Svenska KTH</t>
         </is>
       </c>
       <c r="H10" t="inlineStr">
@@ -762,12 +776,12 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>m.xls</t>
+          <t>Inlämning_Saikat.doc</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>xls</t>
+          <t>doc</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
@@ -777,7 +791,7 @@
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>15360</t>
+          <t>13824</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
@@ -792,7 +806,7 @@
       </c>
       <c r="G11" t="inlineStr">
         <is>
-          <t>TestFiles/subfolder</t>
+          <t>Svenska\Svenska KTH</t>
         </is>
       </c>
       <c r="H11" t="inlineStr">
@@ -814,12 +828,12 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>mm.xls</t>
+          <t>Svenska_Uppg_Novelanalys.doc</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>xls</t>
+          <t>doc</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
@@ -829,7 +843,7 @@
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>15360</t>
+          <t>12800</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
@@ -844,7 +858,7 @@
       </c>
       <c r="G12" t="inlineStr">
         <is>
-          <t>TestFiles/subfolder</t>
+          <t>Svenska</t>
         </is>
       </c>
       <c r="H12" t="inlineStr">
@@ -858,6 +872,1462 @@
         </is>
       </c>
       <c r="J12" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>Svenska_Uppg_Talanalys.doc</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>doc</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>29041</t>
+        </is>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="F13" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="G13" t="inlineStr">
+        <is>
+          <t>Svenska</t>
+        </is>
+      </c>
+      <c r="H13" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="I13" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="J13" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>David Mall för vetenskapligt arbete och gymnasiearbete talanalys (5) (2).docx</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>docx</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>37404</t>
+        </is>
+      </c>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="F14" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="G14" t="inlineStr">
+        <is>
+          <t>Svenska</t>
+        </is>
+      </c>
+      <c r="H14" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="I14" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="J14" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>DELMOMENT språk och makt.docx</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>docx</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>81126</t>
+        </is>
+      </c>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="F15" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="G15" t="inlineStr">
+        <is>
+          <t>Svenska</t>
+        </is>
+      </c>
+      <c r="H15" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="I15" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="J15" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>Källkritik.docx</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>docx</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>15267</t>
+        </is>
+      </c>
+      <c r="E16" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="F16" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="G16" t="inlineStr">
+        <is>
+          <t>Svenska</t>
+        </is>
+      </c>
+      <c r="H16" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="I16" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="J16" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>NOVELL ANALYS SVA3.docx</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>docx</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>25611</t>
+        </is>
+      </c>
+      <c r="E17" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="F17" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="G17" t="inlineStr">
+        <is>
+          <t>Svenska</t>
+        </is>
+      </c>
+      <c r="H17" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="I17" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="J17" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>Novell Maskrosen.docx</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>docx</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>15635</t>
+        </is>
+      </c>
+      <c r="E18" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="F18" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="G18" t="inlineStr">
+        <is>
+          <t>Svenska</t>
+        </is>
+      </c>
+      <c r="H18" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="I18" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="J18" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>Noveller ordförståelse.docx</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>docx</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="D19" t="inlineStr">
+        <is>
+          <t>14957</t>
+        </is>
+      </c>
+      <c r="E19" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="F19" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="G19" t="inlineStr">
+        <is>
+          <t>Svenska</t>
+        </is>
+      </c>
+      <c r="H19" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="I19" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="J19" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>Retorik examin info.docx</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>docx</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="D20" t="inlineStr">
+        <is>
+          <t>16063</t>
+        </is>
+      </c>
+      <c r="E20" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="F20" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="G20" t="inlineStr">
+        <is>
+          <t>Svenska</t>
+        </is>
+      </c>
+      <c r="H20" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="I20" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="J20" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>Symbolism in The Glass Menagerie by H.docx</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>docx</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="D21" t="inlineStr">
+        <is>
+          <t>29758</t>
+        </is>
+      </c>
+      <c r="E21" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="F21" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="G21" t="inlineStr">
+        <is>
+          <t>Svenska</t>
+        </is>
+      </c>
+      <c r="H21" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="I21" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="J21" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>Writing assignment the glass menagerie.docx</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>docx</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="D22" t="inlineStr">
+        <is>
+          <t>19608</t>
+        </is>
+      </c>
+      <c r="E22" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="F22" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="G22" t="inlineStr">
+        <is>
+          <t>Svenska</t>
+        </is>
+      </c>
+      <c r="H22" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="I22" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="J22" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>DropboxInstaller.exe</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>exe</t>
+        </is>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="D23" t="inlineStr">
+        <is>
+          <t>317608</t>
+        </is>
+      </c>
+      <c r="E23" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="F23" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="G23" t="inlineStr">
+        <is>
+          <t>Svenska</t>
+        </is>
+      </c>
+      <c r="H23" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="I23" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="J23" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>5886848-origpic-4d5fe5.gif</t>
+        </is>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>gif</t>
+        </is>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="D24" t="inlineStr">
+        <is>
+          <t>11947</t>
+        </is>
+      </c>
+      <c r="E24" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="F24" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="G24" t="inlineStr">
+        <is>
+          <t>Svenska</t>
+        </is>
+      </c>
+      <c r="H24" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="I24" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="J24" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>zbalph.gif</t>
+        </is>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>gif</t>
+        </is>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="D25" t="inlineStr">
+        <is>
+          <t>14058</t>
+        </is>
+      </c>
+      <c r="E25" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="F25" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="G25" t="inlineStr">
+        <is>
+          <t>Svenska</t>
+        </is>
+      </c>
+      <c r="H25" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="I25" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="J25" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>learn-arabic-letters-alphabet-image-clipart-picture-1.jpg</t>
+        </is>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>jpg</t>
+        </is>
+      </c>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="D26" t="inlineStr">
+        <is>
+          <t>1465823</t>
+        </is>
+      </c>
+      <c r="E26" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="F26" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="G26" t="inlineStr">
+        <is>
+          <t>Svenska</t>
+        </is>
+      </c>
+      <c r="H26" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="I26" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="J26" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>spraktradet.jpg</t>
+        </is>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>jpg</t>
+        </is>
+      </c>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="D27" t="inlineStr">
+        <is>
+          <t>831991</t>
+        </is>
+      </c>
+      <c r="E27" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="F27" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="G27" t="inlineStr">
+        <is>
+          <t>Svenska</t>
+        </is>
+      </c>
+      <c r="H27" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="I27" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="J27" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>Argumenter_och_motargumenter.odt</t>
+        </is>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>odt</t>
+        </is>
+      </c>
+      <c r="C28" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="D28" t="inlineStr">
+        <is>
+          <t>11060</t>
+        </is>
+      </c>
+      <c r="E28" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="F28" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="G28" t="inlineStr">
+        <is>
+          <t>Svenska</t>
+        </is>
+      </c>
+      <c r="H28" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="I28" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="J28" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>Namnlös 1.odt</t>
+        </is>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>odt</t>
+        </is>
+      </c>
+      <c r="C29" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="D29" t="inlineStr">
+        <is>
+          <t>11656</t>
+        </is>
+      </c>
+      <c r="E29" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="F29" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="G29" t="inlineStr">
+        <is>
+          <t>Svenska</t>
+        </is>
+      </c>
+      <c r="H29" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="I29" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="J29" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>Namnlös 2.odt</t>
+        </is>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>odt</t>
+        </is>
+      </c>
+      <c r="C30" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="D30" t="inlineStr">
+        <is>
+          <t>31826</t>
+        </is>
+      </c>
+      <c r="E30" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="F30" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="G30" t="inlineStr">
+        <is>
+          <t>Svenska</t>
+        </is>
+      </c>
+      <c r="H30" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="I30" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="J30" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>Novell_Analys_V2.odt</t>
+        </is>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>odt</t>
+        </is>
+      </c>
+      <c r="C31" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="D31" t="inlineStr">
+        <is>
+          <t>24104</t>
+        </is>
+      </c>
+      <c r="E31" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="F31" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="G31" t="inlineStr">
+        <is>
+          <t>Svenska</t>
+        </is>
+      </c>
+      <c r="H31" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="I31" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="J31" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="inlineStr">
+        <is>
+          <t>Svenska_text.odt</t>
+        </is>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>odt</t>
+        </is>
+      </c>
+      <c r="C32" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="D32" t="inlineStr">
+        <is>
+          <t>29810</t>
+        </is>
+      </c>
+      <c r="E32" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="F32" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="G32" t="inlineStr">
+        <is>
+          <t>Svenska</t>
+        </is>
+      </c>
+      <c r="H32" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="I32" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="J32" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="inlineStr">
+        <is>
+          <t>Svenska_uppg.odt</t>
+        </is>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>odt</t>
+        </is>
+      </c>
+      <c r="C33" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="D33" t="inlineStr">
+        <is>
+          <t>10008</t>
+        </is>
+      </c>
+      <c r="E33" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="F33" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="G33" t="inlineStr">
+        <is>
+          <t>Svenska</t>
+        </is>
+      </c>
+      <c r="H33" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="I33" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="J33" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="inlineStr">
+        <is>
+          <t>Analys-Maskrosen-av-Margit-Bethlen---Novell-42629.pdf</t>
+        </is>
+      </c>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>pdf</t>
+        </is>
+      </c>
+      <c r="C34" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="D34" t="inlineStr">
+        <is>
+          <t>84516</t>
+        </is>
+      </c>
+      <c r="E34" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="F34" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="G34" t="inlineStr">
+        <is>
+          <t>Svenska</t>
+        </is>
+      </c>
+      <c r="H34" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="I34" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="J34" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="inlineStr">
+        <is>
+          <t>Ejercicios_examen_Atom_campos_grav_elect_magnet.pdf</t>
+        </is>
+      </c>
+      <c r="B35" t="inlineStr">
+        <is>
+          <t>pdf</t>
+        </is>
+      </c>
+      <c r="C35" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="D35" t="inlineStr">
+        <is>
+          <t>90704</t>
+        </is>
+      </c>
+      <c r="E35" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="F35" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="G35" t="inlineStr">
+        <is>
+          <t>Svenska</t>
+        </is>
+      </c>
+      <c r="H35" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="I35" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="J35" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="inlineStr">
+        <is>
+          <t>Namnlös 1.ppt</t>
+        </is>
+      </c>
+      <c r="B36" t="inlineStr">
+        <is>
+          <t>ppt</t>
+        </is>
+      </c>
+      <c r="C36" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="D36" t="inlineStr">
+        <is>
+          <t>153088</t>
+        </is>
+      </c>
+      <c r="E36" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="F36" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="G36" t="inlineStr">
+        <is>
+          <t>Svenska</t>
+        </is>
+      </c>
+      <c r="H36" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="I36" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="J36" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="inlineStr">
+        <is>
+          <t>Svenska_NP14_PPT.ppt</t>
+        </is>
+      </c>
+      <c r="B37" t="inlineStr">
+        <is>
+          <t>ppt</t>
+        </is>
+      </c>
+      <c r="C37" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="D37" t="inlineStr">
+        <is>
+          <t>2457088</t>
+        </is>
+      </c>
+      <c r="E37" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="F37" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="G37" t="inlineStr">
+        <is>
+          <t>Svenska</t>
+        </is>
+      </c>
+      <c r="H37" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="I37" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="J37" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="inlineStr">
+        <is>
+          <t>ece68e63e58dbfb840ff33bd9f27d8f0.sdx</t>
+        </is>
+      </c>
+      <c r="B38" t="inlineStr">
+        <is>
+          <t>sdx</t>
+        </is>
+      </c>
+      <c r="C38" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="D38" t="inlineStr">
+        <is>
+          <t>25296</t>
+        </is>
+      </c>
+      <c r="E38" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="F38" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="G38" t="inlineStr">
+        <is>
+          <t>Svenska</t>
+        </is>
+      </c>
+      <c r="H38" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="I38" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="J38" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="inlineStr">
+        <is>
+          <t>ÅÄÖ.txt</t>
+        </is>
+      </c>
+      <c r="B39" t="inlineStr">
+        <is>
+          <t>txt</t>
+        </is>
+      </c>
+      <c r="C39" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="D39" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="E39" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="F39" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="G39" t="inlineStr">
+        <is>
+          <t>Svenska</t>
+        </is>
+      </c>
+      <c r="H39" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="I39" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="J39" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="inlineStr">
+        <is>
+          <t>ÅåÄäÖö.txt</t>
+        </is>
+      </c>
+      <c r="B40" t="inlineStr">
+        <is>
+          <t>txt</t>
+        </is>
+      </c>
+      <c r="C40" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="D40" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="E40" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="F40" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="G40" t="inlineStr">
+        <is>
+          <t>Svenska</t>
+        </is>
+      </c>
+      <c r="H40" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="I40" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="J40" t="inlineStr">
         <is>
           <t/>
         </is>

</xml_diff>

<commit_message>
second sheet locked and unlocked for specified cells
</commit_message>
<xml_diff>
--- a/testfile2.xlsx
+++ b/testfile2.xlsx
@@ -259,7 +259,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="9.0" state="frozen" topLeftCell="A10" activePane="bottomLeft"/>
+      <selection pane="bottomLeft"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0"/>
   <sheetData>
@@ -315,8 +318,8 @@
         </is>
       </c>
     </row>
-    <row r="2" s="4" customFormat="1">
-      <c r="A2" t="inlineStr">
+    <row r="2">
+      <c r="A2" s="4" t="inlineStr">
         <is>
           <t>.DS_Store</t>
         </is>
@@ -367,13 +370,13 @@
         </is>
       </c>
     </row>
-    <row r="3" s="4" customFormat="1">
+    <row r="3">
       <c r="A3" t="inlineStr">
         <is>
           <t>.DS_Store</t>
         </is>
       </c>
-      <c r="B3" t="inlineStr">
+      <c r="B3" s="4" t="inlineStr">
         <is>
           <t>DS_Store</t>
         </is>
@@ -419,7 +422,7 @@
         </is>
       </c>
     </row>
-    <row r="4" s="4" customFormat="1">
+    <row r="4">
       <c r="A4" t="inlineStr">
         <is>
           <t>.DS_Store</t>
@@ -430,7 +433,7 @@
           <t>DS_Store</t>
         </is>
       </c>
-      <c r="C4" t="inlineStr">
+      <c r="C4" s="4" t="inlineStr">
         <is>
           <t/>
         </is>
@@ -471,7 +474,7 @@
         </is>
       </c>
     </row>
-    <row r="5" s="4" customFormat="1">
+    <row r="5">
       <c r="A5" t="inlineStr">
         <is>
           <t>Harry_Potter_and_the_Goblet_of_Fire_2005.mkv</t>
@@ -487,7 +490,7 @@
           <t/>
         </is>
       </c>
-      <c r="D5" t="inlineStr">
+      <c r="D5" s="4" t="inlineStr">
         <is>
           <t>443051505</t>
         </is>
@@ -523,7 +526,7 @@
         </is>
       </c>
     </row>
-    <row r="6" s="4" customFormat="1">
+    <row r="6">
       <c r="A6" t="inlineStr">
         <is>
           <t>Lucifer.S02E04.HDTV.x264-LOL[eztv].mkv</t>
@@ -544,7 +547,7 @@
           <t>324677395</t>
         </is>
       </c>
-      <c r="E6" t="inlineStr">
+      <c r="E6" s="4" t="inlineStr">
         <is>
           <t/>
         </is>
@@ -575,7 +578,7 @@
         </is>
       </c>
     </row>
-    <row r="7" s="4" customFormat="1">
+    <row r="7">
       <c r="A7" t="inlineStr">
         <is>
           <t>Skaermavbild_2018-02-19_kl._22.57.05.png</t>
@@ -601,7 +604,7 @@
           <t/>
         </is>
       </c>
-      <c r="F7" t="inlineStr">
+      <c r="F7" s="4" t="inlineStr">
         <is>
           <t/>
         </is>
@@ -627,7 +630,7 @@
         </is>
       </c>
     </row>
-    <row r="8" s="4" customFormat="1">
+    <row r="8">
       <c r="A8" t="inlineStr">
         <is>
           <t>AEAEAEAEAE.txt</t>
@@ -658,7 +661,7 @@
           <t/>
         </is>
       </c>
-      <c r="G8" t="inlineStr">
+      <c r="G8" s="4" t="inlineStr">
         <is>
           <t>TestFiles</t>
         </is>
@@ -679,7 +682,7 @@
         </is>
       </c>
     </row>
-    <row r="9" s="4" customFormat="1">
+    <row r="9">
       <c r="A9" t="inlineStr">
         <is>
           <t>aaaaaaaaaa.txt</t>
@@ -715,7 +718,7 @@
           <t>TestFiles/OE/aa</t>
         </is>
       </c>
-      <c r="H9" t="inlineStr">
+      <c r="H9" s="4" t="inlineStr">
         <is>
           <t/>
         </is>
@@ -731,7 +734,7 @@
         </is>
       </c>
     </row>
-    <row r="10" s="4" customFormat="1">
+    <row r="10">
       <c r="A10" t="inlineStr">
         <is>
           <t>oeaeoeaeoeaeoeae.txt</t>
@@ -772,7 +775,7 @@
           <t/>
         </is>
       </c>
-      <c r="I10" t="inlineStr">
+      <c r="I10" s="4" t="inlineStr">
         <is>
           <t/>
         </is>
@@ -783,7 +786,7 @@
         </is>
       </c>
     </row>
-    <row r="11" s="4" customFormat="1">
+    <row r="11">
       <c r="A11" t="inlineStr">
         <is>
           <t>m.xls</t>
@@ -829,13 +832,13 @@
           <t/>
         </is>
       </c>
-      <c r="J11" t="inlineStr">
-        <is>
-          <t/>
-        </is>
-      </c>
-    </row>
-    <row r="12" s="4" customFormat="1">
+      <c r="J11" s="4" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+    </row>
+    <row r="12">
       <c r="A12" t="inlineStr">
         <is>
           <t>mm.xls</t>

</xml_diff>

<commit_message>
Second sheet proteced except cells under content
</commit_message>
<xml_diff>
--- a/testfile2.xlsx
+++ b/testfile2.xlsx
@@ -66,10 +66,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="true"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <protection locked="false"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="true"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <protection locked="false"/>
@@ -104,7 +107,11 @@
           <t>Riksarkivets diarienummer leveransöverenskommelse</t>
         </is>
       </c>
-      <c r="B2"/>
+      <c r="B2" s="3" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
@@ -112,7 +119,11 @@
           <t>Riksarkivets diarienummer leverans</t>
         </is>
       </c>
-      <c r="B3"/>
+      <c r="B3" s="3" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
     </row>
     <row r="4">
       <c r="A4" s="2" t="inlineStr">
@@ -120,7 +131,11 @@
           <t>Beskrivning av leveransen</t>
         </is>
       </c>
-      <c r="B4"/>
+      <c r="B4" s="3" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
     </row>
     <row r="5">
       <c r="A5" s="2" t="inlineStr">
@@ -128,7 +143,11 @@
           <t>Arkivbildare</t>
         </is>
       </c>
-      <c r="B5"/>
+      <c r="B5" s="3" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
     </row>
     <row r="6">
       <c r="A6" s="2" t="inlineStr">
@@ -136,7 +155,11 @@
           <t>Organisationsnummer arkivbildare</t>
         </is>
       </c>
-      <c r="B6"/>
+      <c r="B6" s="3" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
     </row>
     <row r="7">
       <c r="A7" s="2" t="inlineStr">
@@ -144,7 +167,11 @@
           <t>Levererande myndighet</t>
         </is>
       </c>
-      <c r="B7"/>
+      <c r="B7" s="3" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
     </row>
     <row r="8">
       <c r="A8" s="2" t="inlineStr">
@@ -152,7 +179,11 @@
           <t>Organisationsnummer levererande myndighet</t>
         </is>
       </c>
-      <c r="B8"/>
+      <c r="B8" s="3" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
     </row>
     <row r="9">
       <c r="A9" s="2" t="inlineStr">
@@ -160,7 +191,11 @@
           <t>Servicebyrå/Konsult</t>
         </is>
       </c>
-      <c r="B9"/>
+      <c r="B9" s="3" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
     </row>
     <row r="10">
       <c r="A10" s="2" t="inlineStr">
@@ -168,7 +203,11 @@
           <t>Kontaktperson för leverans</t>
         </is>
       </c>
-      <c r="B10"/>
+      <c r="B10" s="3" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
     </row>
     <row r="11">
       <c r="A11" s="2" t="inlineStr">
@@ -176,7 +215,11 @@
           <t>Telefonnummer till kontaktperson</t>
         </is>
       </c>
-      <c r="B11"/>
+      <c r="B11" s="3" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
     </row>
     <row r="12">
       <c r="A12" s="2" t="inlineStr">
@@ -184,7 +227,11 @@
           <t>Kostnadsställe</t>
         </is>
       </c>
-      <c r="B12"/>
+      <c r="B12" s="3" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
     </row>
     <row r="13">
       <c r="A13" s="1" t="inlineStr">
@@ -192,7 +239,11 @@
           <t>Kontaktperson för e-fakturering</t>
         </is>
       </c>
-      <c r="B13"/>
+      <c r="B13" s="3" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
     </row>
     <row r="14">
       <c r="A14" s="1" t="inlineStr">
@@ -200,7 +251,11 @@
           <t>Arkivets namn</t>
         </is>
       </c>
-      <c r="B14"/>
+      <c r="B14" s="3" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
     </row>
     <row r="15">
       <c r="A15" s="2" t="inlineStr">
@@ -208,7 +263,11 @@
           <t>Systemets namn</t>
         </is>
       </c>
-      <c r="B15"/>
+      <c r="B15" s="3" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
     </row>
     <row r="16">
       <c r="A16" s="2" t="inlineStr">
@@ -216,7 +275,11 @@
           <t>Uttagsdatum</t>
         </is>
       </c>
-      <c r="B16"/>
+      <c r="B16" s="3" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
     </row>
     <row r="17">
       <c r="A17" s="2" t="inlineStr">
@@ -224,7 +287,11 @@
           <t>Kommentar</t>
         </is>
       </c>
-      <c r="B17"/>
+      <c r="B17" s="3" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
     </row>
     <row r="18">
       <c r="A18" s="2" t="inlineStr">
@@ -232,7 +299,11 @@
           <t>Projektkod</t>
         </is>
       </c>
-      <c r="B18"/>
+      <c r="B18" s="3" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
     </row>
     <row r="19">
       <c r="A19" s="1" t="inlineStr">
@@ -240,7 +311,11 @@
           <t>Accessions-ID</t>
         </is>
       </c>
-      <c r="B19"/>
+      <c r="B19" s="3" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
     </row>
     <row r="20">
       <c r="A20" s="1" t="inlineStr">
@@ -248,9 +323,14 @@
           <t>Batch-ID</t>
         </is>
       </c>
-      <c r="B20"/>
+      <c r="B20" s="3" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
     </row>
   </sheetData>
+  <sheetProtection password="0000" sheet="true" scenarios="true" objects="true"/>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
@@ -267,624 +347,624 @@
   <sheetFormatPr defaultRowHeight="15.0"/>
   <sheetData>
     <row r="1">
-      <c r="A1" s="3" t="inlineStr">
+      <c r="A1" s="4" t="inlineStr">
         <is>
           <t>FILNAMN</t>
         </is>
       </c>
-      <c r="B1" s="3" t="inlineStr">
+      <c r="B1" s="4" t="inlineStr">
         <is>
           <t>FILTYP</t>
         </is>
       </c>
-      <c r="C1" s="3" t="inlineStr">
+      <c r="C1" s="4" t="inlineStr">
         <is>
           <t>FILTYPSVERSION</t>
         </is>
       </c>
-      <c r="D1" s="3" t="inlineStr">
+      <c r="D1" s="4" t="inlineStr">
         <is>
           <t>STORLEK (Bytes)</t>
         </is>
       </c>
-      <c r="E1" s="3" t="inlineStr">
+      <c r="E1" s="4" t="inlineStr">
         <is>
           <t>TECKENUPPSÄTTNING</t>
         </is>
       </c>
-      <c r="F1" s="3" t="inlineStr">
+      <c r="F1" s="4" t="inlineStr">
         <is>
           <t>SPELTID (endast audio och video)</t>
         </is>
       </c>
-      <c r="G1" s="3" t="inlineStr">
+      <c r="G1" s="4" t="inlineStr">
         <is>
           <t>SÖKVÄG (path, url)</t>
         </is>
       </c>
-      <c r="H1" s="3" t="inlineStr">
+      <c r="H1" s="4" t="inlineStr">
         <is>
           <t>SEKRETESSGRAD HOS MYNDIGHETEN</t>
         </is>
       </c>
-      <c r="I1" s="3" t="inlineStr">
+      <c r="I1" s="4" t="inlineStr">
         <is>
           <t>BEHANDLING AV PERSONUPPGIFTER</t>
         </is>
       </c>
-      <c r="J1" s="3" t="inlineStr">
+      <c r="J1" s="4" t="inlineStr">
         <is>
           <t>KOMMENTAR</t>
         </is>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="4" t="inlineStr">
+      <c r="A2" s="5" t="inlineStr">
         <is>
           <t>.DS_Store</t>
         </is>
       </c>
-      <c r="B2" t="inlineStr">
+      <c r="B2" s="5" t="inlineStr">
         <is>
           <t>DS_Store</t>
         </is>
       </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t/>
-        </is>
-      </c>
-      <c r="D2" t="inlineStr">
+      <c r="C2" s="5" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="D2" s="5" t="inlineStr">
         <is>
           <t>8196</t>
         </is>
       </c>
-      <c r="E2" t="inlineStr">
-        <is>
-          <t/>
-        </is>
-      </c>
-      <c r="F2" t="inlineStr">
-        <is>
-          <t/>
-        </is>
-      </c>
-      <c r="G2" t="inlineStr">
+      <c r="E2" s="5" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="F2" s="5" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="G2" s="5" t="inlineStr">
         <is>
           <t>TestFiles</t>
         </is>
       </c>
-      <c r="H2" t="inlineStr">
-        <is>
-          <t/>
-        </is>
-      </c>
-      <c r="I2" t="inlineStr">
-        <is>
-          <t/>
-        </is>
-      </c>
-      <c r="J2" t="inlineStr">
+      <c r="H2" s="5" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="I2" s="5" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="J2" s="5" t="inlineStr">
         <is>
           <t/>
         </is>
       </c>
     </row>
     <row r="3">
-      <c r="A3" t="inlineStr">
+      <c r="A3" s="5" t="inlineStr">
         <is>
           <t>.DS_Store</t>
         </is>
       </c>
-      <c r="B3" s="4" t="inlineStr">
+      <c r="B3" s="5" t="inlineStr">
         <is>
           <t>DS_Store</t>
         </is>
       </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t/>
-        </is>
-      </c>
-      <c r="D3" t="inlineStr">
+      <c r="C3" s="5" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="D3" s="5" t="inlineStr">
         <is>
           <t>6148</t>
         </is>
       </c>
-      <c r="E3" t="inlineStr">
-        <is>
-          <t/>
-        </is>
-      </c>
-      <c r="F3" t="inlineStr">
-        <is>
-          <t/>
-        </is>
-      </c>
-      <c r="G3" t="inlineStr">
+      <c r="E3" s="5" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="F3" s="5" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="G3" s="5" t="inlineStr">
         <is>
           <t>TestFiles/OE</t>
         </is>
       </c>
-      <c r="H3" t="inlineStr">
-        <is>
-          <t/>
-        </is>
-      </c>
-      <c r="I3" t="inlineStr">
-        <is>
-          <t/>
-        </is>
-      </c>
-      <c r="J3" t="inlineStr">
+      <c r="H3" s="5" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="I3" s="5" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="J3" s="5" t="inlineStr">
         <is>
           <t/>
         </is>
       </c>
     </row>
     <row r="4">
-      <c r="A4" t="inlineStr">
+      <c r="A4" s="5" t="inlineStr">
         <is>
           <t>.DS_Store</t>
         </is>
       </c>
-      <c r="B4" t="inlineStr">
+      <c r="B4" s="5" t="inlineStr">
         <is>
           <t>DS_Store</t>
         </is>
       </c>
-      <c r="C4" s="4" t="inlineStr">
-        <is>
-          <t/>
-        </is>
-      </c>
-      <c r="D4" t="inlineStr">
+      <c r="C4" s="5" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="D4" s="5" t="inlineStr">
         <is>
           <t>6148</t>
         </is>
       </c>
-      <c r="E4" t="inlineStr">
-        <is>
-          <t/>
-        </is>
-      </c>
-      <c r="F4" t="inlineStr">
-        <is>
-          <t/>
-        </is>
-      </c>
-      <c r="G4" t="inlineStr">
+      <c r="E4" s="5" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="F4" s="5" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="G4" s="5" t="inlineStr">
         <is>
           <t>TestFiles/subfolder</t>
         </is>
       </c>
-      <c r="H4" t="inlineStr">
-        <is>
-          <t/>
-        </is>
-      </c>
-      <c r="I4" t="inlineStr">
-        <is>
-          <t/>
-        </is>
-      </c>
-      <c r="J4" t="inlineStr">
+      <c r="H4" s="5" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="I4" s="5" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="J4" s="5" t="inlineStr">
         <is>
           <t/>
         </is>
       </c>
     </row>
     <row r="5">
-      <c r="A5" t="inlineStr">
+      <c r="A5" s="5" t="inlineStr">
         <is>
           <t>Harry_Potter_and_the_Goblet_of_Fire_2005.mkv</t>
         </is>
       </c>
-      <c r="B5" t="inlineStr">
+      <c r="B5" s="5" t="inlineStr">
         <is>
           <t>mkv</t>
         </is>
       </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t/>
-        </is>
-      </c>
-      <c r="D5" s="4" t="inlineStr">
+      <c r="C5" s="5" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="D5" s="5" t="inlineStr">
         <is>
           <t>443051505</t>
         </is>
       </c>
-      <c r="E5" t="inlineStr">
-        <is>
-          <t/>
-        </is>
-      </c>
-      <c r="F5" t="inlineStr">
+      <c r="E5" s="5" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="F5" s="5" t="inlineStr">
         <is>
           <t>02:37:06</t>
         </is>
       </c>
-      <c r="G5" t="inlineStr">
+      <c r="G5" s="5" t="inlineStr">
         <is>
           <t>TestFiles/movies</t>
         </is>
       </c>
-      <c r="H5" t="inlineStr">
-        <is>
-          <t/>
-        </is>
-      </c>
-      <c r="I5" t="inlineStr">
-        <is>
-          <t/>
-        </is>
-      </c>
-      <c r="J5" t="inlineStr">
+      <c r="H5" s="5" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="I5" s="5" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="J5" s="5" t="inlineStr">
         <is>
           <t/>
         </is>
       </c>
     </row>
     <row r="6">
-      <c r="A6" t="inlineStr">
+      <c r="A6" s="5" t="inlineStr">
         <is>
           <t>Lucifer.S02E04.HDTV.x264-LOL[eztv].mkv</t>
         </is>
       </c>
-      <c r="B6" t="inlineStr">
+      <c r="B6" s="5" t="inlineStr">
         <is>
           <t>mkv</t>
         </is>
       </c>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t/>
-        </is>
-      </c>
-      <c r="D6" t="inlineStr">
+      <c r="C6" s="5" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="D6" s="5" t="inlineStr">
         <is>
           <t>324677395</t>
         </is>
       </c>
-      <c r="E6" s="4" t="inlineStr">
-        <is>
-          <t/>
-        </is>
-      </c>
-      <c r="F6" t="inlineStr">
+      <c r="E6" s="5" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="F6" s="5" t="inlineStr">
         <is>
           <t>00:42:15</t>
         </is>
       </c>
-      <c r="G6" t="inlineStr">
+      <c r="G6" s="5" t="inlineStr">
         <is>
           <t>TestFiles/movies</t>
         </is>
       </c>
-      <c r="H6" t="inlineStr">
-        <is>
-          <t/>
-        </is>
-      </c>
-      <c r="I6" t="inlineStr">
-        <is>
-          <t/>
-        </is>
-      </c>
-      <c r="J6" t="inlineStr">
+      <c r="H6" s="5" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="I6" s="5" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="J6" s="5" t="inlineStr">
         <is>
           <t/>
         </is>
       </c>
     </row>
     <row r="7">
-      <c r="A7" t="inlineStr">
+      <c r="A7" s="5" t="inlineStr">
         <is>
           <t>Skaermavbild_2018-02-19_kl._22.57.05.png</t>
         </is>
       </c>
-      <c r="B7" t="inlineStr">
+      <c r="B7" s="5" t="inlineStr">
         <is>
           <t>png</t>
         </is>
       </c>
-      <c r="C7" t="inlineStr">
-        <is>
-          <t/>
-        </is>
-      </c>
-      <c r="D7" t="inlineStr">
+      <c r="C7" s="5" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="D7" s="5" t="inlineStr">
         <is>
           <t>2460165</t>
         </is>
       </c>
-      <c r="E7" t="inlineStr">
-        <is>
-          <t/>
-        </is>
-      </c>
-      <c r="F7" s="4" t="inlineStr">
-        <is>
-          <t/>
-        </is>
-      </c>
-      <c r="G7" t="inlineStr">
+      <c r="E7" s="5" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="F7" s="5" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="G7" s="5" t="inlineStr">
         <is>
           <t>TestFiles/subfolder/another_subfolder</t>
         </is>
       </c>
-      <c r="H7" t="inlineStr">
-        <is>
-          <t/>
-        </is>
-      </c>
-      <c r="I7" t="inlineStr">
-        <is>
-          <t/>
-        </is>
-      </c>
-      <c r="J7" t="inlineStr">
+      <c r="H7" s="5" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="I7" s="5" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="J7" s="5" t="inlineStr">
         <is>
           <t/>
         </is>
       </c>
     </row>
     <row r="8">
-      <c r="A8" t="inlineStr">
+      <c r="A8" s="5" t="inlineStr">
         <is>
           <t>AEAEAEAEAE.txt</t>
         </is>
       </c>
-      <c r="B8" t="inlineStr">
+      <c r="B8" s="5" t="inlineStr">
         <is>
           <t>txt</t>
         </is>
       </c>
-      <c r="C8" t="inlineStr">
-        <is>
-          <t/>
-        </is>
-      </c>
-      <c r="D8" t="inlineStr">
+      <c r="C8" s="5" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="D8" s="5" t="inlineStr">
         <is>
           <t>5</t>
         </is>
       </c>
-      <c r="E8" t="inlineStr">
+      <c r="E8" s="5" t="inlineStr">
         <is>
           <t>UTF-8</t>
         </is>
       </c>
-      <c r="F8" t="inlineStr">
-        <is>
-          <t/>
-        </is>
-      </c>
-      <c r="G8" s="4" t="inlineStr">
+      <c r="F8" s="5" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="G8" s="5" t="inlineStr">
         <is>
           <t>TestFiles</t>
         </is>
       </c>
-      <c r="H8" t="inlineStr">
-        <is>
-          <t/>
-        </is>
-      </c>
-      <c r="I8" t="inlineStr">
-        <is>
-          <t/>
-        </is>
-      </c>
-      <c r="J8" t="inlineStr">
+      <c r="H8" s="5" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="I8" s="5" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="J8" s="5" t="inlineStr">
         <is>
           <t/>
         </is>
       </c>
     </row>
     <row r="9">
-      <c r="A9" t="inlineStr">
+      <c r="A9" s="5" t="inlineStr">
         <is>
           <t>aaaaaaaaaa.txt</t>
         </is>
       </c>
-      <c r="B9" t="inlineStr">
+      <c r="B9" s="5" t="inlineStr">
         <is>
           <t>txt</t>
         </is>
       </c>
-      <c r="C9" t="inlineStr">
-        <is>
-          <t/>
-        </is>
-      </c>
-      <c r="D9" t="inlineStr">
+      <c r="C9" s="5" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="D9" s="5" t="inlineStr">
         <is>
           <t>27</t>
         </is>
       </c>
-      <c r="E9" t="inlineStr">
+      <c r="E9" s="5" t="inlineStr">
         <is>
           <t>UTF-8</t>
         </is>
       </c>
-      <c r="F9" t="inlineStr">
-        <is>
-          <t/>
-        </is>
-      </c>
-      <c r="G9" t="inlineStr">
+      <c r="F9" s="5" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="G9" s="5" t="inlineStr">
         <is>
           <t>TestFiles/OE/aa</t>
         </is>
       </c>
-      <c r="H9" s="4" t="inlineStr">
-        <is>
-          <t/>
-        </is>
-      </c>
-      <c r="I9" t="inlineStr">
-        <is>
-          <t/>
-        </is>
-      </c>
-      <c r="J9" t="inlineStr">
+      <c r="H9" s="5" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="I9" s="5" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="J9" s="5" t="inlineStr">
         <is>
           <t/>
         </is>
       </c>
     </row>
     <row r="10">
-      <c r="A10" t="inlineStr">
+      <c r="A10" s="5" t="inlineStr">
         <is>
           <t>oeaeoeaeoeaeoeae.txt</t>
         </is>
       </c>
-      <c r="B10" t="inlineStr">
+      <c r="B10" s="5" t="inlineStr">
         <is>
           <t>txt</t>
         </is>
       </c>
-      <c r="C10" t="inlineStr">
-        <is>
-          <t/>
-        </is>
-      </c>
-      <c r="D10" t="inlineStr">
+      <c r="C10" s="5" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="D10" s="5" t="inlineStr">
         <is>
           <t>22</t>
         </is>
       </c>
-      <c r="E10" t="inlineStr">
+      <c r="E10" s="5" t="inlineStr">
         <is>
           <t>UTF-8</t>
         </is>
       </c>
-      <c r="F10" t="inlineStr">
-        <is>
-          <t/>
-        </is>
-      </c>
-      <c r="G10" t="inlineStr">
+      <c r="F10" s="5" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="G10" s="5" t="inlineStr">
         <is>
           <t>TestFiles/OE</t>
         </is>
       </c>
-      <c r="H10" t="inlineStr">
-        <is>
-          <t/>
-        </is>
-      </c>
-      <c r="I10" s="4" t="inlineStr">
-        <is>
-          <t/>
-        </is>
-      </c>
-      <c r="J10" t="inlineStr">
+      <c r="H10" s="5" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="I10" s="5" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="J10" s="5" t="inlineStr">
         <is>
           <t/>
         </is>
       </c>
     </row>
     <row r="11">
-      <c r="A11" t="inlineStr">
+      <c r="A11" s="5" t="inlineStr">
         <is>
           <t>m.xls</t>
         </is>
       </c>
-      <c r="B11" t="inlineStr">
+      <c r="B11" s="5" t="inlineStr">
         <is>
           <t>xls</t>
         </is>
       </c>
-      <c r="C11" t="inlineStr">
-        <is>
-          <t/>
-        </is>
-      </c>
-      <c r="D11" t="inlineStr">
+      <c r="C11" s="5" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="D11" s="5" t="inlineStr">
         <is>
           <t>15360</t>
         </is>
       </c>
-      <c r="E11" t="inlineStr">
-        <is>
-          <t/>
-        </is>
-      </c>
-      <c r="F11" t="inlineStr">
-        <is>
-          <t/>
-        </is>
-      </c>
-      <c r="G11" t="inlineStr">
+      <c r="E11" s="5" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="F11" s="5" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="G11" s="5" t="inlineStr">
         <is>
           <t>TestFiles/subfolder</t>
         </is>
       </c>
-      <c r="H11" t="inlineStr">
-        <is>
-          <t/>
-        </is>
-      </c>
-      <c r="I11" t="inlineStr">
-        <is>
-          <t/>
-        </is>
-      </c>
-      <c r="J11" s="4" t="inlineStr">
+      <c r="H11" s="5" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="I11" s="5" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="J11" s="5" t="inlineStr">
         <is>
           <t/>
         </is>
       </c>
     </row>
     <row r="12">
-      <c r="A12" t="inlineStr">
+      <c r="A12" s="5" t="inlineStr">
         <is>
           <t>mm.xls</t>
         </is>
       </c>
-      <c r="B12" t="inlineStr">
+      <c r="B12" s="5" t="inlineStr">
         <is>
           <t>xls</t>
         </is>
       </c>
-      <c r="C12" t="inlineStr">
-        <is>
-          <t/>
-        </is>
-      </c>
-      <c r="D12" t="inlineStr">
+      <c r="C12" s="5" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="D12" s="5" t="inlineStr">
         <is>
           <t>15360</t>
         </is>
       </c>
-      <c r="E12" t="inlineStr">
-        <is>
-          <t/>
-        </is>
-      </c>
-      <c r="F12" t="inlineStr">
-        <is>
-          <t/>
-        </is>
-      </c>
-      <c r="G12" t="inlineStr">
+      <c r="E12" s="5" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="F12" s="5" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="G12" s="5" t="inlineStr">
         <is>
           <t>TestFiles/subfolder</t>
         </is>
       </c>
-      <c r="H12" t="inlineStr">
-        <is>
-          <t/>
-        </is>
-      </c>
-      <c r="I12" t="inlineStr">
-        <is>
-          <t/>
-        </is>
-      </c>
-      <c r="J12" t="inlineStr">
+      <c r="H12" s="5" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="I12" s="5" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="J12" s="5" t="inlineStr">
         <is>
           <t/>
         </is>

</xml_diff>